<commit_message>
🧐 Cargar datos de tasas con la corrección condicional por debajo de base #204
</commit_message>
<xml_diff>
--- a/aplicaciones/www/estaticos/datos/descarga/ya2-5-marco-integral.xlsx
+++ b/aplicaciones/www/estaticos/datos/descarga/ya2-5-marco-integral.xlsx
@@ -10,10 +10,21 @@
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>

</xml_diff>